<commit_message>
New HTMLS and table structure updated
</commit_message>
<xml_diff>
--- a/all_tables.xlsx
+++ b/all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28021"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Scraping\Web-Scraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Web Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{482EEB6F-FC14-46C3-90D1-FF6660FB5567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7C8193-F6D6-439E-9384-4A7CDBC0F49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{1E3576A2-3D48-48ED-A989-302ABCBD99E1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{1E3576A2-3D48-48ED-A989-302ABCBD99E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <author>Dibyajyoti Parida</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{E51E7AB1-A5D3-462F-9536-2388BD056F0B}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{E51E7AB1-A5D3-462F-9536-2388BD056F0B}">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{95EE722C-E05D-4D29-B166-8D31DA2BFACC}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{95EE722C-E05D-4D29-B166-8D31DA2BFACC}">
       <text>
         <r>
           <rPr>
@@ -94,6 +94,595 @@
  18 Aug 2024 01:44 UTC
 17 Aug 2024 21:44 Local
 Store only the UTC date</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{AF1A6041-78C0-4C9A-8DDA-42D5E0E8CD00}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{25E8FA25-EC47-42A4-8556-04B82C88874D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sort by desc</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{9BDFEEBF-13C5-4F80-A4A5-2C45C995146C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Delete this column</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{61F56B65-FAD1-468E-A533-081E638B5208}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Separate into two columns in silver layer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{3DDF22DE-AB14-43B6-95C7-A1BD2474A6E5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Intensity Rating</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{7DC05EDB-ED75-4CA2-A115-61B393982D06}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Radius and Intensity are alternatively available
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{460BFE1D-1E24-44A1-8229-BD5D613057C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip this</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{4DC7A82F-A11E-4E7F-B3AA-B045E0E10BCB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip this</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{829A59A4-FE1C-40BC-9BEC-0B59CC7AC2C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Segregate this in Silver Layer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{409E5A4C-1816-4D2D-B988-C155DD42C195}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{5C4A8DB5-CA00-4A58-8575-7C6095CA5E2F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip this in gold layer using aggregation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{6F08F19B-CC0D-470A-87BD-DDA8C9BE98AF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip this in Gold layer using aggregation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{5AAC9BBA-EAE8-4D7F-9317-2833214FA166}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip this in bronze layer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{CBBD9709-34A6-4629-8E48-7370F05EEDC8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip in golden layer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{DD30637B-DAB8-454C-95DD-1439581A7DC7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip in golden layer</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dibyajyoti Parida</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{F5DE4D8D-871D-4CDD-A403-6102779C71A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Segregate this in Silver Layer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{B2F88E3A-BBDA-46A8-9B09-299CE7AA0CFD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ 18 Aug 2024 01:44 UTC
+17 Aug 2024 21:44 Local
+Store only the UTC date</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{F2D14B1D-34DB-4EB5-8286-8A2CD1080DBE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sort by desc</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{65912160-CC8A-4AB9-A1AA-B41E595AA016}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Delete this column</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00DB409A-A113-450A-81B5-09EB280C2E2A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip this in gold layer using aggregation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{2750FEA9-1AC3-4C9A-938B-4B2358537D09}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip this in Gold layer using aggregation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{034221B4-0216-4182-A2F9-7785D076EDF3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip this in bronze layer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{1D36015A-E170-45C1-8069-C80F3A14A74B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip in golden layer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G23" authorId="0" shapeId="0" xr:uid="{A25D8BFE-68A9-4D69-91E8-EC5651F1C85B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dibyajyoti Parida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip in golden layer</t>
         </r>
       </text>
     </comment>
@@ -102,7 +691,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
   <si>
     <t>Cy</t>
   </si>
@@ -135,13 +724,202 @@
   </si>
   <si>
     <t>Table 2</t>
+  </si>
+  <si>
+    <t>Impact Timeline</t>
+  </si>
+  <si>
+    <t>GDACS Score</t>
+  </si>
+  <si>
+    <t>Population Affected</t>
+  </si>
+  <si>
+    <t>Burned Area</t>
+  </si>
+  <si>
+    <t>Last Update</t>
+  </si>
+  <si>
+    <t>GWIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID </t>
+  </si>
+  <si>
+    <t>Alert Color</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>Exposed population</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Affected Provinces</t>
+  </si>
+  <si>
+    <t>Region Province</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>City class</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Table 5</t>
+  </si>
+  <si>
+    <t>Affected populated places</t>
+  </si>
+  <si>
+    <t>Airports</t>
+  </si>
+  <si>
+    <t>Ports</t>
+  </si>
+  <si>
+    <t>Dams</t>
+  </si>
+  <si>
+    <t>IATA Code</t>
+  </si>
+  <si>
+    <t>Elevation (m)</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Runway type</t>
+  </si>
+  <si>
+    <t>IFR</t>
+  </si>
+  <si>
+    <t>Runway Length (ft)</t>
+  </si>
+  <si>
+    <t>LOCODE</t>
+  </si>
+  <si>
+    <t>Reservoir</t>
+  </si>
+  <si>
+    <t>Dam Name</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Inserted at:</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Mag, Depth</t>
+  </si>
+  <si>
+    <t>MMI*</t>
+  </si>
+  <si>
+    <t>Population**</t>
+  </si>
+  <si>
+    <t>Tsunami risk***</t>
+  </si>
+  <si>
+    <t>Delay (hh:mm)</t>
+  </si>
+  <si>
+    <t>Episode Timeline</t>
+  </si>
+  <si>
+    <t>Table 6</t>
+  </si>
+  <si>
+    <t>Table 7</t>
+  </si>
+  <si>
+    <t>Table 8</t>
+  </si>
+  <si>
+    <t>Table 9</t>
+  </si>
+  <si>
+    <t>Table 10</t>
+  </si>
+  <si>
+    <t>Nuclear power plants</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Radius/Intensity</t>
+  </si>
+  <si>
+    <t>Shakemaps Timeline</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>Shake id #</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>episodeid</t>
+  </si>
+  <si>
+    <t>Lat/Lon</t>
+  </si>
+  <si>
+    <t>Max MMI</t>
+  </si>
+  <si>
+    <t>Date shake (UTC)</t>
+  </si>
+  <si>
+    <t>Can fetch the Image element for the shakemap using title of the element</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +939,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -535,58 +1326,376 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EA2CC6-4AEC-422F-B36C-AC0BC009CEF1}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -594,7 +1703,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2092BC19-237A-4CFA-9C31-D56E3373F39C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -645,13 +1756,291 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CC374C-CA42-41BD-8DC5-0B71A4427A93}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CC374C-CA42-41BD-8DC5-0B71A4427A93}">
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified the code to include script and created Py.ipynb is complete for Wildfires
</commit_message>
<xml_diff>
--- a/all_tables.xlsx
+++ b/all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Scraping\Web-Scraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Web Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E29A33-77B2-4539-9548-E4E59783CF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D614D27-106F-4EC0-A117-F29311000132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{1E3576A2-3D48-48ED-A989-302ABCBD99E1}"/>
+    <workbookView xWindow="-2892" yWindow="12852" windowWidth="23256" windowHeight="13176" activeTab="6" xr2:uid="{1E3576A2-3D48-48ED-A989-302ABCBD99E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -316,11 +316,20 @@
     </comment>
     <comment ref="M11" authorId="1" shapeId="0" xr:uid="{CEAAC038-C14E-4936-BF00-8F65B333F8C2}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Skip
 </t>
+        </r>
       </text>
     </comment>
     <comment ref="D17" authorId="0" shapeId="0" xr:uid="{5C4A8DB5-CA00-4A58-8575-7C6095CA5E2F}">
@@ -973,7 +982,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="125">
   <si>
     <t>Table 1</t>
   </si>
@@ -1321,6 +1330,33 @@
   </si>
   <si>
     <t>Populated places</t>
+  </si>
+  <si>
+    <t>Main Table</t>
+  </si>
+  <si>
+    <t>Event type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL </t>
+  </si>
+  <si>
+    <t>Start_date/last_detected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People affected </t>
+  </si>
+  <si>
+    <t>Burned area</t>
+  </si>
+  <si>
+    <t>More info</t>
+  </si>
+  <si>
+    <t>Nuclear Power Plant</t>
+  </si>
+  <si>
+    <t>Reactors</t>
   </si>
 </sst>
 </file>
@@ -1741,12 +1777,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A80ABD-0B4B-4163-9F37-30CF1522B302}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1756,7 +1814,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:K21"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2340,7 +2398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C14AEC-B5A7-4CCA-9C06-CB80FFB21F09}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -2821,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CC374C-CA42-41BD-8DC5-0B71A4427A93}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2833,8 +2891,8 @@
     <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -2850,22 +2908,22 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2929,7 +2987,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -2954,7 +3012,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
@@ -2988,7 +3046,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
@@ -3028,7 +3086,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
@@ -3056,7 +3114,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
         <v>33</v>
@@ -3085,20 +3143,32 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>